<commit_message>
plotting results & policy attribution
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c46ea174191bacb1/Documenti/LAURA/HERTIE 22-23/THESIS/patent_breakdetection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86AEDDDA-C9D0-461B-B3F8-7F0F3B7450EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{86AEDDDA-C9D0-461B-B3F8-7F0F3B7450EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E17C3EA-EA4B-456D-9313-1E790D801602}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{036FC188-B32F-4E45-814C-E20E670B38F0}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11235" activeTab="1" xr2:uid="{036FC188-B32F-4E45-814C-E20E670B38F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -238,7 +239,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="173" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -359,9 +360,9 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
@@ -689,17 +690,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C238A857-8519-4EB3-9682-D70F5DA35E6C}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -728,7 +729,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -757,7 +758,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -786,7 +787,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -815,7 +816,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -844,7 +845,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
@@ -873,7 +874,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -902,7 +903,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
@@ -931,7 +932,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
@@ -960,12 +961,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>31</v>
       </c>
@@ -994,7 +995,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>39</v>
       </c>
@@ -1023,7 +1024,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>40</v>
       </c>
@@ -1052,7 +1053,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>41</v>
       </c>
@@ -1081,7 +1082,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>42</v>
       </c>
@@ -1110,7 +1111,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>47</v>
       </c>
@@ -1136,7 +1137,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>48</v>
       </c>
@@ -1162,7 +1163,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>49</v>
       </c>
@@ -1188,7 +1189,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>54</v>
       </c>
@@ -1217,7 +1218,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>60</v>
       </c>
@@ -1243,7 +1244,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>61</v>
       </c>
@@ -1269,7 +1270,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -1279,4 +1280,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF6D02A0-3786-4408-8631-B742E40156BE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
clean and document code
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c46ea174191bacb1/Documenti/LAURA/HERTIE 22-23/THESIS/patent_breakdetection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{86AEDDDA-C9D0-461B-B3F8-7F0F3B7450EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{700C9F76-05E5-4FE2-BC76-E3FB21F6785A}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{86AEDDDA-C9D0-461B-B3F8-7F0F3B7450EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C97B288-BCB3-4D59-88B4-67ACD07C835B}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11235" xr2:uid="{036FC188-B32F-4E45-814C-E20E670B38F0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{036FC188-B32F-4E45-814C-E20E670B38F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
   <si>
     <t>country</t>
   </si>
@@ -65,9 +65,6 @@
     <t>tci</t>
   </si>
   <si>
-    <t>0.0006812 ***</t>
-  </si>
-  <si>
     <t xml:space="preserve">Wisconsin  </t>
   </si>
   <si>
@@ -164,42 +161,9 @@
     <t>"log_patent_count ~ lgdp + lpop + lgdp_sq " us_q30       2000:2019   0.01  AR:4</t>
   </si>
   <si>
-    <t xml:space="preserve"> Formula: log_patent_count ~ lgdp + lpop + lgdp_sq + lfuel  us_q30 (2000:2019); p.value: 0.01; AR: 0 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0070323 **   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> California  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.0062540 **      </t>
-  </si>
-  <si>
-    <t>Michigan</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Formula: log_patent_count ~ lgdp + lpop + lgdp_sq + lfuel  us_q30 (2000:2019); p.value: 0.01; AR: 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Formula: log_patent_count ~ lgdp + lpop + lgdp_sq + lfuel  us_q30 (2000:2019); p.value: 0.01; AR: 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Formula: log_patent_count ~ lgdp + lpop + lgdp_sq + lfuel  us_q30 (2000:2019); p.value: 0.01; AR: 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.167e-11 ***  </t>
-  </si>
-  <si>
     <t>SouthCarolina</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0003474 ***   </t>
-  </si>
-  <si>
-    <t>Wisconsin</t>
-  </si>
-  <si>
     <t xml:space="preserve">Formula: ihs_patent_count ~ lgdp + lpop + lgdp_sq + avg_temp    us_q30 (2000:2019); p.value: 0.01; AR: 0        </t>
   </si>
   <si>
@@ -222,6 +186,9 @@
   </si>
   <si>
     <t>Formula: ihs_patent_count ~ lgdp + lpop + lgdp_sq + avg_temp    us_q30 (2000:2019); p.value: 0.01; AR: 2</t>
+  </si>
+  <si>
+    <t>\</t>
   </si>
 </sst>
 </file>
@@ -261,7 +228,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -292,12 +259,6 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -323,15 +284,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -339,14 +299,11 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -357,15 +314,13 @@
     </xf>
     <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="5" borderId="0" xfId="4" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="1" fillId="6" borderId="0" xfId="5" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="5">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="20% - Accent2" xfId="2" builtinId="34"/>
     <cellStyle name="20% - Accent3" xfId="3" builtinId="38"/>
     <cellStyle name="20% - Accent4" xfId="4" builtinId="42"/>
-    <cellStyle name="20% - Accent6" xfId="5" builtinId="50"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -682,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C238A857-8519-4EB3-9682-D70F5DA35E6C}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,7 +651,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -717,29 +672,29 @@
         <v>8</v>
       </c>
       <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
         <v>11</v>
-      </c>
-      <c r="I1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="1">
         <v>2008</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="11">
         <v>0.78681400000000001</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="11">
         <v>0.11632099999999999</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="14" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="1">
@@ -749,27 +704,27 @@
         <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>10</v>
+      <c r="B3" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="C3" s="1">
         <v>2014</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="11">
         <v>0.41981600000000002</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="11">
         <v>0.122979</v>
       </c>
-      <c r="F3" s="17" t="s">
-        <v>9</v>
+      <c r="F3" s="14" t="s">
+        <v>50</v>
       </c>
       <c r="G3" s="1">
         <v>7</v>
@@ -778,27 +733,27 @@
         <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>16</v>
+      <c r="B4" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="C4" s="2">
         <v>2008</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="12">
         <v>0.79278470000000001</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="12">
         <v>0.1216131</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G4" s="2">
         <v>2</v>
@@ -807,7 +762,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -815,19 +770,19 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2">
         <v>2011</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="12">
         <v>1.183775</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="12">
         <v>0.17772260000000001</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G5" s="2">
         <v>1</v>
@@ -836,27 +791,27 @@
         <v>0</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2">
         <v>2007</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="12">
         <v>1.1599666</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="12">
         <v>0.27102130000000002</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G6" s="2">
         <v>1</v>
@@ -865,27 +820,27 @@
         <v>0</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2">
         <v>2005</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="12">
         <v>0.4845546</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="12">
         <v>0.13525409999999999</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G7" s="2">
         <v>5</v>
@@ -894,27 +849,27 @@
         <v>0</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>10</v>
+        <v>25</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="C8" s="2">
         <v>2014</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="13">
         <v>0.42323349999999998</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="12">
         <v>0.12833049999999999</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G8" s="2">
         <v>7</v>
@@ -923,27 +878,27 @@
         <v>0</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="C9" s="2">
         <v>2005</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="12">
         <v>0.412159</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="12">
         <v>0.13544639999999999</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G9" s="2">
         <v>8</v>
@@ -952,32 +907,32 @@
         <v>0</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="4">
         <v>2011</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="15">
         <v>1.1046872000000001</v>
       </c>
       <c r="E11" s="4">
         <v>0.17094909999999999</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G11" s="4">
         <v>1</v>
@@ -986,27 +941,27 @@
         <v>1</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="4">
         <v>2019</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="15">
         <v>0.68189339999999998</v>
       </c>
       <c r="E12" s="4">
         <v>0.2570461</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G12" s="4">
         <v>2</v>
@@ -1015,27 +970,27 @@
         <v>1</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="C13" s="4">
         <v>2008</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="15">
         <v>0.73182910000000001</v>
       </c>
       <c r="E13" s="4">
         <v>0.1227253</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G13" s="4">
         <v>2</v>
@@ -1044,27 +999,27 @@
         <v>1</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="C14" s="4">
         <v>2014</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="15">
         <v>0.41864990000000002</v>
       </c>
       <c r="E14" s="4">
         <v>0.1244092</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G14" s="4">
         <v>7</v>
@@ -1073,191 +1028,95 @@
         <v>1</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>42</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="5">
+        <v>2002</v>
+      </c>
+      <c r="D15" s="16">
+        <v>0.77365189999999995</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0.21162210000000001</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="5">
-        <v>2006</v>
-      </c>
-      <c r="D15" s="19">
-        <v>0.37307200000000001</v>
-      </c>
-      <c r="E15" s="5">
-        <v>0.13796700000000001</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>43</v>
+      <c r="G15" s="5">
+        <v>2</v>
       </c>
       <c r="H15" s="5">
         <v>0</v>
       </c>
-      <c r="I15" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J15" s="8"/>
-    </row>
-    <row r="16" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="1:10" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="C16" s="5">
-        <v>2003</v>
-      </c>
-      <c r="D16" s="19">
-        <v>0.44035600000000003</v>
+        <v>2008</v>
+      </c>
+      <c r="D16" s="16">
+        <v>0.83062429999999998</v>
       </c>
       <c r="E16" s="5">
-        <v>0.160523</v>
+        <v>0.12877949999999999</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="G16" s="5">
+        <v>2</v>
       </c>
       <c r="H16" s="5">
         <v>0</v>
       </c>
-      <c r="I16" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I16" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="C17" s="5">
-        <v>2008</v>
-      </c>
-      <c r="D17" s="19">
-        <v>0.76921399999999995</v>
+        <v>2014</v>
+      </c>
+      <c r="D17" s="16">
+        <v>0.4548084</v>
       </c>
       <c r="E17" s="5">
-        <v>0.11561200000000001</v>
+        <v>0.13687540000000001</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="G17" s="5">
+        <v>7</v>
       </c>
       <c r="H17" s="5">
         <v>0</v>
       </c>
-      <c r="I17" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="5">
-        <v>2014</v>
-      </c>
-      <c r="D18" s="19">
-        <v>0.43841599999999997</v>
-      </c>
-      <c r="E18" s="5">
-        <v>0.12189899999999999</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H18" s="5">
-        <v>0</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="6">
-        <v>2002</v>
-      </c>
-      <c r="D19" s="20">
-        <v>0.77365189999999995</v>
-      </c>
-      <c r="E19" s="6">
-        <v>0.21162210000000001</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H19" s="6">
-        <v>0</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="J19" s="7"/>
-    </row>
-    <row r="20" spans="1:10" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="6">
-        <v>2008</v>
-      </c>
-      <c r="D20" s="20">
-        <v>0.83062429999999998</v>
-      </c>
-      <c r="E20" s="6">
-        <v>0.12877949999999999</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H20" s="6">
-        <v>0</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="6">
-        <v>2014</v>
-      </c>
-      <c r="D21" s="20">
-        <v>0.4548084</v>
-      </c>
-      <c r="E21" s="6">
-        <v>0.13687540000000001</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="H21" s="6">
-        <v>0</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>13</v>
+      <c r="I17" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>